<commit_message>
Adding Contacts XL, POM and TSc
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/contacts.xlsx
+++ b/src/main/resources/excel/contacts.xlsx
@@ -1,26 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11340" windowHeight="2925"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Barbara</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>LoginPageText</t>
+  </si>
+  <si>
+    <t>vtiger</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Administrator</t>
+  </si>
+  <si>
+    <t>UserDropDownOption</t>
+  </si>
+  <si>
+    <t>Navya</t>
+  </si>
+  <si>
+    <t>TextWhenNotPresent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                 No Contact Found !
+          </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,8 +89,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -111,7 +154,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -146,7 +189,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -323,20 +366,68 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="60">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
duplicate contacts test scripts, contacts pom page,contacts excel file,homepage
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/contacts.xlsx
+++ b/src/main/resources/excel/contacts.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{149D7D81-DB74-46EF-A7A6-5B68D5178A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11340" windowHeight="2925"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="11364" windowHeight="4380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:H15"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="38">
   <si>
     <t>FirstName</t>
   </si>
@@ -54,13 +57,94 @@
     <t xml:space="preserve">
                  No Contact Found !
           </t>
+  </si>
+  <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Criteria</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Expected Page</t>
+  </si>
+  <si>
+    <t>VTIG-117</t>
+  </si>
+  <si>
+    <t>TY_117</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Are you sure you want to delete the selected</t>
+  </si>
+  <si>
+    <t>xyz@gmail.com</t>
+  </si>
+  <si>
+    <t>123@gmail.com</t>
+  </si>
+  <si>
+    <t>VTIG-118</t>
+  </si>
+  <si>
+    <t>TY_118</t>
+  </si>
+  <si>
+    <t>Select atleast two records for merging</t>
+  </si>
+  <si>
+    <t>Duplicate Contacts</t>
+  </si>
+  <si>
+    <t>VTIG-119</t>
+  </si>
+  <si>
+    <t>TY_119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you sure you want to delete the selected </t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>VTIG-120</t>
+  </si>
+  <si>
+    <t>TY_120</t>
+  </si>
+  <si>
+    <t>VTIG-121</t>
+  </si>
+  <si>
+    <t>TY_121</t>
+  </si>
+  <si>
+    <t>VTIG-122</t>
+  </si>
+  <si>
+    <t>TY_122</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,16 +152,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -85,17 +182,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -366,28 +504,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60">
+    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -425,6 +563,402 @@
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="38.21875" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="4">
+        <v>8888888120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E19" s="5"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DeleteDuplicate TestScripts, updated Contacts PoM page, updated contacts excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/contacts.xlsx
+++ b/src/main/resources/excel/contacts.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11340" windowHeight="2925"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11340" windowHeight="2928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="38">
   <si>
     <t>FirstName</t>
   </si>
@@ -54,13 +55,94 @@
     <t xml:space="preserve">
                  No Contact Found !
           </t>
+  </si>
+  <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Criteria</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Expected Page</t>
+  </si>
+  <si>
+    <t>VTIG-117</t>
+  </si>
+  <si>
+    <t>TY_117</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Are you sure you want to delete the selected</t>
+  </si>
+  <si>
+    <t>xyz@gmail.com</t>
+  </si>
+  <si>
+    <t>123@gmail.com</t>
+  </si>
+  <si>
+    <t>VTIG-118</t>
+  </si>
+  <si>
+    <t>TY_118</t>
+  </si>
+  <si>
+    <t>Select atleast two records for merging</t>
+  </si>
+  <si>
+    <t>Duplicate Contacts</t>
+  </si>
+  <si>
+    <t>VTIG-119</t>
+  </si>
+  <si>
+    <t>TY_119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you sure you want to delete the selected </t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>VTIG-120</t>
+  </si>
+  <si>
+    <t>TY_120</t>
+  </si>
+  <si>
+    <t>VTIG-121</t>
+  </si>
+  <si>
+    <t>TY_121</t>
+  </si>
+  <si>
+    <t>VTIG-122</t>
+  </si>
+  <si>
+    <t>TY_122</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,16 +150,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -85,17 +180,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -366,7 +502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -376,15 +512,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -407,7 +543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60">
+    <row r="2" spans="1:6" ht="57.6">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -425,6 +561,400 @@
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="38.21875" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1"/>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1"/>
+    <row r="11" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1"/>
+    <row r="16" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1">
+      <c r="A16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="4">
+        <v>8888888120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="E19" s="5"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1"/>
+    <row r="21" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1">
+      <c r="A21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15" thickBot="1"/>
+    <row r="26" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>